<commit_message>
fixed maintenance, adding MTTF capability
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/test_PM.xlsx
+++ b/shipClassTests/testResults/test_PM.xlsx
@@ -462,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1039,10 +1039,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1072,10 +1072,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1084,10 +1084,10 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1105,10 +1105,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1117,10 +1117,10 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1138,10 +1138,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1150,10 +1150,10 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1171,10 +1171,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1183,10 +1183,10 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1204,10 +1204,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1216,10 +1216,10 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1237,10 +1237,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1249,10 +1249,10 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1270,10 +1270,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1282,10 +1282,10 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1303,10 +1303,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1315,10 +1315,10 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1336,10 +1336,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1765,10 +1765,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1798,10 +1798,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1810,10 +1810,10 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -1831,10 +1831,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1843,10 +1843,10 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -1864,10 +1864,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1876,10 +1876,10 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -1897,10 +1897,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1909,10 +1909,10 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -1930,10 +1930,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1942,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2095,10 +2095,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2107,10 +2107,10 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -2123,8 +2123,173 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>-1</v>
+      </c>
+      <c r="C51">
+        <v>-1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" s="4">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>-1</v>
+      </c>
+      <c r="G51">
+        <v>-1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>1</v>
+      </c>
+      <c r="J51" s="3">
+        <f>IF(B51 = F51, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>-1</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" s="4">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>-1</v>
+      </c>
+      <c r="G52">
+        <v>-1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" s="4">
+        <v>1</v>
+      </c>
+      <c r="J52" s="3">
+        <f>IF(B52 = F52, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>-1</v>
+      </c>
+      <c r="C53">
+        <v>-1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>-1</v>
+      </c>
+      <c r="G53">
+        <v>-1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3">
+        <f>IF(B53 = F53, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>-1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>-1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <f>IF(B54 = F54, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <f>IF(B55 = F55, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J50">
+  <conditionalFormatting sqref="J2:J55">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2140,7 +2305,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2275,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2312,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2380,10 +2545,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -2417,10 +2582,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -2454,10 +2619,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -2491,10 +2656,10 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -2784,7 +2949,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2821,28 +2986,28 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E19" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I19" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J19" s="3">
         <f>IF(B19 = F19, 1, 0)</f>
@@ -2858,28 +3023,28 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E20" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I20" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J20" s="3">
         <f>IF(B20 = F20, 1, 0)</f>
@@ -2895,28 +3060,28 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E21" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I21" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J21" s="3">
         <f>IF(B21 = F21, 1, 0)</f>
@@ -2932,28 +3097,28 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E22" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I22" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J22" s="3">
         <f>IF(B22 = F22, 1, 0)</f>
@@ -2969,28 +3134,28 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E23" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I23" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J23" s="3">
         <f>IF(B23 = F23, 1, 0)</f>
@@ -3006,28 +3171,28 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E24" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I24" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J24" s="3">
         <f>IF(B24 = F24, 1, 0)</f>
@@ -3043,28 +3208,28 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E25" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I25" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J25" s="3">
         <f>IF(B25 = F25, 1, 0)</f>
@@ -3080,28 +3245,28 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E26" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I26" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J26" s="3">
         <f>IF(B26 = F26, 1, 0)</f>
@@ -3117,28 +3282,28 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E27" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I27" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J27" s="3">
         <f>IF(B27 = F27, 1, 0)</f>
@@ -3157,13 +3322,13 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -3194,13 +3359,13 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -3231,13 +3396,13 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -3268,13 +3433,13 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -3305,13 +3470,13 @@
         <v>1</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -3342,13 +3507,13 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -3379,13 +3544,13 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -3416,13 +3581,13 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3453,13 +3618,13 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3490,13 +3655,13 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -3527,7 +3692,7 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -3564,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -3598,10 +3763,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -3635,28 +3800,28 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I41" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J41" s="3">
         <f>IF(B41 = F41, 1, 0)</f>
@@ -3672,28 +3837,28 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I42" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J42" s="3">
         <f>IF(B42 = F42, 1, 0)</f>
@@ -3709,28 +3874,28 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I43" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J43" s="3">
         <f>IF(B43 = F43, 1, 0)</f>
@@ -3746,28 +3911,28 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I44" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J44" s="3">
         <f>IF(B44 = F44, 1, 0)</f>
@@ -3783,28 +3948,28 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I45" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J45" s="3">
         <f>IF(B45 = F45, 1, 0)</f>
@@ -3968,28 +4133,28 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E50" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I50" s="4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J50" s="3">
         <f>IF(B50 = F50, 1, 0)</f>
@@ -4000,8 +4165,230 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>-1</v>
+      </c>
+      <c r="C51">
+        <v>-1</v>
+      </c>
+      <c r="D51">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F51">
+        <v>-1</v>
+      </c>
+      <c r="G51">
+        <v>-1</v>
+      </c>
+      <c r="H51">
+        <v>-1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J51" s="3">
+        <f>IF(B51 = F51, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
+        <f>MODE(C51:E51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>-1</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+      <c r="D52">
+        <v>-1</v>
+      </c>
+      <c r="E52" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F52">
+        <v>-1</v>
+      </c>
+      <c r="G52">
+        <v>-1</v>
+      </c>
+      <c r="H52">
+        <v>-1</v>
+      </c>
+      <c r="I52" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J52" s="3">
+        <f>IF(B52 = F52, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
+        <f>MODE(C52:E52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>-1</v>
+      </c>
+      <c r="C53">
+        <v>-1</v>
+      </c>
+      <c r="D53">
+        <v>-1</v>
+      </c>
+      <c r="E53" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F53">
+        <v>-1</v>
+      </c>
+      <c r="G53">
+        <v>-1</v>
+      </c>
+      <c r="H53">
+        <v>-1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J53" s="3">
+        <f>IF(B53 = F53, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
+        <f>MODE(C53:E53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>-1</v>
+      </c>
+      <c r="C54">
+        <v>-1</v>
+      </c>
+      <c r="D54">
+        <v>-1</v>
+      </c>
+      <c r="E54" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F54">
+        <v>-1</v>
+      </c>
+      <c r="G54">
+        <v>-1</v>
+      </c>
+      <c r="H54">
+        <v>-1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J54" s="3">
+        <f>IF(B54 = F54, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <f>MODE(C54:E54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <f>IF(B55 = F55, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <f>MODE(C55:E55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" s="4">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" s="4">
+        <v>1</v>
+      </c>
+      <c r="J56" s="3">
+        <f>IF(B56 = F56, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <f>MODE(C56:E56)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J50">
+  <conditionalFormatting sqref="J2:J56">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4011,7 +4398,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K50">
+  <conditionalFormatting sqref="K2:K56">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4027,7 +4414,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4119,10 +4506,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -4156,10 +4543,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
@@ -4193,10 +4580,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
@@ -4233,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -4270,7 +4657,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -4307,7 +4694,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -4344,7 +4731,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -4381,7 +4768,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -4418,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -4455,7 +4842,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -4492,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -4529,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -4566,7 +4953,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -4603,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -4640,7 +5027,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="4">
         <v>0</v>
@@ -4677,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -4714,7 +5101,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4">
         <v>0</v>
@@ -4751,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4">
         <v>0</v>
@@ -4788,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -4825,7 +5212,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -4862,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
@@ -4899,7 +5286,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
@@ -4936,7 +5323,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -4973,7 +5360,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
@@ -5010,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -5887,8 +6274,230 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>1</v>
+      </c>
+      <c r="J51" s="3">
+        <f>IF(B51 = F51, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
+        <f>MODE(C51:E51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" s="4">
+        <v>1</v>
+      </c>
+      <c r="J52" s="3">
+        <f>IF(B52 = F52, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
+        <f>MODE(C52:E52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3">
+        <f>IF(B53 = F53, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
+        <f>MODE(C53:E53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="4">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <f>IF(B54 = F54, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <f>MODE(C54:E54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <f>IF(B55 = F55, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <f>MODE(C55:E55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" s="4">
+        <v>1</v>
+      </c>
+      <c r="J56" s="3">
+        <f>IF(B56 = F56, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <f>MODE(C56:E56)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J50">
+  <conditionalFormatting sqref="J2:J56">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -5898,7 +6507,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K50">
+  <conditionalFormatting sqref="K2:K56">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -5914,7 +6523,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6012,7 +6621,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -6046,10 +6655,10 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -6080,13 +6689,13 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -6117,13 +6726,13 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -6154,13 +6763,13 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -6191,13 +6800,13 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -6228,13 +6837,13 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -6265,13 +6874,13 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -6302,13 +6911,13 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -6339,13 +6948,13 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -6379,10 +6988,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -6416,10 +7025,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -6453,10 +7062,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -6490,10 +7099,10 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -7774,8 +8383,230 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>1</v>
+      </c>
+      <c r="J51" s="3">
+        <f>IF(B51 = F51, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
+        <f>MODE(C51:E51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" s="4">
+        <v>1</v>
+      </c>
+      <c r="J52" s="3">
+        <f>IF(B52 = F52, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
+        <f>MODE(C52:E52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3">
+        <f>IF(B53 = F53, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
+        <f>MODE(C53:E53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="4">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <f>IF(B54 = F54, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <f>MODE(C54:E54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <f>IF(B55 = F55, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <f>MODE(C55:E55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" s="4">
+        <v>1</v>
+      </c>
+      <c r="J56" s="3">
+        <f>IF(B56 = F56, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <f>MODE(C56:E56)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J50">
+  <conditionalFormatting sqref="J2:J56">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -7785,7 +8616,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K50">
+  <conditionalFormatting sqref="K2:K56">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>